<commit_message>
adding todays eth price to excel
</commit_message>
<xml_diff>
--- a/example_mining_data.xlsx
+++ b/example_mining_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Mining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEBE6DE1-3CC7-4D21-9A63-FD610FEBB93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FD3096-1C06-4A5A-A8EB-0A7EB6FC4DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4545" yWindow="1305" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="2475" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date:</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Days to next payout:</t>
+  </si>
+  <si>
+    <t>Today's ETH price [USD]:</t>
   </si>
 </sst>
 </file>
@@ -381,15 +384,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
   </cols>
@@ -399,21 +402,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>44512</v>
-      </c>
-      <c r="C1" s="1">
-        <v>44512</v>
-      </c>
+        <v>44515</v>
+      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>179.2</v>
-      </c>
-      <c r="C2">
-        <v>179.2</v>
+        <v>178.9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -421,10 +419,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="C3">
-        <v>3.5999999999999997E-2</v>
+        <v>3.2199999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -432,10 +427,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2.8900000000000002E-3</v>
-      </c>
-      <c r="C4">
-        <v>3.1900000000000001E-3</v>
+        <v>2.96E-3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -445,19 +437,21 @@
       <c r="B5">
         <v>0.65739999999999998</v>
       </c>
-      <c r="C5">
-        <v>0.65739999999999998</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>25</v>
-      </c>
-      <c r="C6">
-        <v>24</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>4609.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>